<commit_message>
Feb 12 Update 2
</commit_message>
<xml_diff>
--- a/Data/StimulusModule.xlsx
+++ b/Data/StimulusModule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenkinnucan/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C27C63E-90BE-2F43-80C1-6BC1C7AA1F55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9788CF28-98EF-1849-85B4-0BBE33A46322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="1360" windowWidth="27640" windowHeight="15900" xr2:uid="{406C51AA-FDA0-BD41-9A68-09D008286824}"/>
+    <workbookView xWindow="32880" yWindow="-2000" windowWidth="27640" windowHeight="15900" xr2:uid="{406C51AA-FDA0-BD41-9A68-09D008286824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Question</t>
   </si>
@@ -256,6 +256,18 @@
       </rPr>
       <t xml:space="preserve"> on? Select all that apply. </t>
     </r>
+  </si>
+  <si>
+    <t>•Food
+•Clothing
+•Household supplies and personal care                                 •Household items (TV, electronics, furniture, appliances)  
+•Recreational goods (sports and fitness equipment, bicycles, toys, games)                             
+•Rent
+•Mortgage                                                                             •Utilities and telecommunications
+•Vehicle payments                                                              •Paying down credit card, student loans, or other debts  
+•Charitable donations or giving to family members                             
+•Savings or other investments
+•Other, please describe:</t>
   </si>
 </sst>
 </file>
@@ -319,19 +331,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -651,205 +666,206 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.1640625" customWidth="1"/>
-    <col min="2" max="2" width="48.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="238" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="136" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="238" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="238" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="E10" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="136" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="106" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="238" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>43</v>
-      </c>
-    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>